<commit_message>
get the result 12.14
</commit_message>
<xml_diff>
--- a/12d_array_result/result3/Copy of GELCODES_SIFE_Oct20.xlsx
+++ b/12d_array_result/result3/Copy of GELCODES_SIFE_Oct20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luoji\Desktop\PythonWorkSpace\GMM\old_ver\12d_array_result\result3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1E0EE3-80E7-4BA2-9A22-60FB5259988E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF8DF70-D5DF-44BF-A11E-F5184E81DF80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="804" yWindow="3648" windowWidth="16860" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7248" yWindow="4656" windowWidth="16860" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="90">
   <si>
     <t>TEST SAMPLES</t>
   </si>
@@ -274,6 +274,36 @@
   </si>
   <si>
     <t>2.jpg</t>
+  </si>
+  <si>
+    <t>[1. 1. 0. 0. 0. 0. 0. 1. 0. 0. 1. 0.]</t>
+  </si>
+  <si>
+    <t>[1. 0. 1. 0. 0. 0. 0. 1. 0. 0. 0. 1.]</t>
+  </si>
+  <si>
+    <t>[1. 0. 0. 1. 0. 0. 0. 0. 1. 0. 1. 0.]</t>
+  </si>
+  <si>
+    <t>[1. 0. 0. 0. 1. 0. 0. 0. 1. 0. 0. 1.]</t>
+  </si>
+  <si>
+    <t>G A M K L</t>
+  </si>
+  <si>
+    <t>[1. 0. 0. 0. 0. 1. 0. 0. 0. 1. 1. 0.]</t>
+  </si>
+  <si>
+    <t>[1. 0. 0. 0. 0. 0. 1. 0. 0. 1. 0. 1.]</t>
+  </si>
+  <si>
+    <t>[1. 0. 0. 0. 0. 0. 0. 0. 0. 0. 1. 0.]</t>
+  </si>
+  <si>
+    <t>[1. 0. 0. 0. 0. 0. 0. 0. 0. 0. 0. 1.]</t>
+  </si>
+  <si>
+    <t>[1. 0. 0. 0. 0. 0. 0. 1. 0. 0. 0. 0.]</t>
   </si>
 </sst>
 </file>
@@ -316,9 +346,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,29 +632,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M193"/>
+  <dimension ref="A1:R193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="11" max="11" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="L1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -638,8 +669,14 @@
       <c r="H2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -657,16 +694,10 @@
         <v>7</v>
       </c>
       <c r="K3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" t="s">
-        <v>70</v>
-      </c>
-      <c r="M3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -684,16 +715,19 @@
         <v>9</v>
       </c>
       <c r="K4" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4" t="s">
         <v>5</v>
       </c>
-      <c r="L4" t="s">
-        <v>72</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
+        <v>70</v>
+      </c>
+      <c r="R4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -711,16 +745,19 @@
         <v>11</v>
       </c>
       <c r="K5" t="s">
+        <v>81</v>
+      </c>
+      <c r="P5" t="s">
         <v>5</v>
       </c>
-      <c r="L5" t="s">
-        <v>73</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="Q5" t="s">
+        <v>72</v>
+      </c>
+      <c r="R5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -738,16 +775,19 @@
         <v>13</v>
       </c>
       <c r="K6" t="s">
+        <v>82</v>
+      </c>
+      <c r="P6" t="s">
         <v>5</v>
       </c>
-      <c r="L6" t="s">
-        <v>74</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="Q6" t="s">
+        <v>73</v>
+      </c>
+      <c r="R6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -765,16 +805,19 @@
         <v>15</v>
       </c>
       <c r="K7" t="s">
+        <v>83</v>
+      </c>
+      <c r="P7" t="s">
         <v>5</v>
       </c>
-      <c r="L7" t="s">
-        <v>75</v>
-      </c>
-      <c r="M7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="Q7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -792,16 +835,19 @@
         <v>17</v>
       </c>
       <c r="K8" t="s">
+        <v>85</v>
+      </c>
+      <c r="P8" t="s">
         <v>5</v>
       </c>
-      <c r="L8" t="s">
-        <v>77</v>
-      </c>
-      <c r="M8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="Q8" t="s">
+        <v>75</v>
+      </c>
+      <c r="R8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -819,16 +865,19 @@
         <v>19</v>
       </c>
       <c r="K9" t="s">
+        <v>86</v>
+      </c>
+      <c r="P9" t="s">
         <v>5</v>
       </c>
-      <c r="L9" t="s">
-        <v>78</v>
-      </c>
-      <c r="M9" t="s">
+      <c r="Q9" t="s">
+        <v>77</v>
+      </c>
+      <c r="R9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -846,16 +895,19 @@
         <v>21</v>
       </c>
       <c r="K10" t="s">
+        <v>87</v>
+      </c>
+      <c r="P10" t="s">
         <v>5</v>
       </c>
-      <c r="L10" t="s">
-        <v>79</v>
-      </c>
-      <c r="M10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="Q10" t="s">
+        <v>78</v>
+      </c>
+      <c r="R10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -872,8 +924,20 @@
       <c r="H11" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K11" t="s">
+        <v>88</v>
+      </c>
+      <c r="P11" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>79</v>
+      </c>
+      <c r="R11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -890,8 +954,11 @@
       <c r="H12" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -903,7 +970,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -921,7 +988,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -939,7 +1006,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
read all data from excel
</commit_message>
<xml_diff>
--- a/12d_array_result/result3/Copy of GELCODES_SIFE_Oct20.xlsx
+++ b/12d_array_result/result3/Copy of GELCODES_SIFE_Oct20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luoji\Desktop\PythonWorkSpace\GMM\old_ver\12d_array_result\result3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E3B72F-9E78-401E-9B26-3AE26C3D9C9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95B3BA6-181C-42B6-8A80-5373FBFDE84F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6864" yWindow="3540" windowWidth="16860" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -329,12 +329,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -349,12 +355,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,7 +645,7 @@
   <dimension ref="A1:R193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,13 +1068,13 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="3">
         <v>1018</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="1"/>
@@ -1229,13 +1236,13 @@
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="3">
         <v>1032</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="1"/>
@@ -2117,13 +2124,13 @@
       <c r="D107" s="1"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
+      <c r="A108" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="3">
         <v>1106</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D108" s="1"/>
@@ -3151,23 +3158,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Classification xmlns="98201be9-bed6-4c9e-8a9b-8dbdcb59b52e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD172B1A8CFBF549BD23145C0D4C69AA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60d392b449e0a1bb062ed007359ef7f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="98201be9-bed6-4c9e-8a9b-8dbdcb59b52e" xmlns:ns4="eb7b1eea-95e0-4f99-a517-75d51ebb206f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f35683e864675bf732228debc427d31" ns3:_="" ns4:_="">
     <xsd:import namespace="98201be9-bed6-4c9e-8a9b-8dbdcb59b52e"/>
@@ -3396,32 +3386,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DC39010-99A4-420F-8930-47F0BD8B70E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE820B19-5BD7-4D43-B454-CB6C3816E5A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="eb7b1eea-95e0-4f99-a517-75d51ebb206f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="98201be9-bed6-4c9e-8a9b-8dbdcb59b52e"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Classification xmlns="98201be9-bed6-4c9e-8a9b-8dbdcb59b52e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA519E84-2031-44C1-A446-0F69C93EE441}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3438,4 +3420,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DC39010-99A4-420F-8930-47F0BD8B70E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE820B19-5BD7-4D43-B454-CB6C3816E5A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="eb7b1eea-95e0-4f99-a517-75d51ebb206f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="98201be9-bed6-4c9e-8a9b-8dbdcb59b52e"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
finalize all the result yahoo!
</commit_message>
<xml_diff>
--- a/12d_array_result/result3/Copy of GELCODES_SIFE_Oct20.xlsx
+++ b/12d_array_result/result3/Copy of GELCODES_SIFE_Oct20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luoji\Desktop\PythonWorkSpace\GMM\old_ver\12d_array_result\result3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96FDFA9-A61B-46AE-9CB2-CBE517055B2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF35875B-08F8-492D-BAA7-611BD013CFEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15372" yWindow="2016" windowWidth="13164" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="2088" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D193" sqref="D193"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1111,13 +1111,13 @@
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="4">
         <v>1021</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="1"/>
@@ -2131,13 +2131,13 @@
       <c r="D107" s="1"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B108" s="3">
+      <c r="B108" s="4">
         <v>1106</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C108" s="4" t="s">
         <v>55</v>
       </c>
       <c r="D108" s="1"/>
@@ -3165,15 +3165,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD172B1A8CFBF549BD23145C0D4C69AA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60d392b449e0a1bb062ed007359ef7f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="98201be9-bed6-4c9e-8a9b-8dbdcb59b52e" xmlns:ns4="eb7b1eea-95e0-4f99-a517-75d51ebb206f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f35683e864675bf732228debc427d31" ns3:_="" ns4:_="">
     <xsd:import namespace="98201be9-bed6-4c9e-8a9b-8dbdcb59b52e"/>
@@ -3402,6 +3393,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3411,14 +3411,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DC39010-99A4-420F-8930-47F0BD8B70E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA519E84-2031-44C1-A446-0F69C93EE441}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3433,6 +3425,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DC39010-99A4-420F-8930-47F0BD8B70E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
create label keys and values with pickle
</commit_message>
<xml_diff>
--- a/12d_array_result/result3/Copy of GELCODES_SIFE_Oct20.xlsx
+++ b/12d_array_result/result3/Copy of GELCODES_SIFE_Oct20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luoji\Desktop\PythonWorkSpace\GMM\old_ver\12d_array_result\result3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF35875B-08F8-492D-BAA7-611BD013CFEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52139B2-855E-46D4-B4F9-75E64EAC18D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="2088" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="91">
   <si>
     <t>TEST SAMPLES</t>
   </si>
@@ -329,18 +329,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -361,14 +355,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R193"/>
+  <dimension ref="A1:R191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,14 +1068,14 @@
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="3">
-        <v>1018</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>14</v>
+      <c r="B20" s="1">
+        <v>1019</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1091,7 +1084,7 @@
         <v>31</v>
       </c>
       <c r="B21" s="1">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
@@ -1099,50 +1092,50 @@
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="1">
-        <v>1020</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
+      <c r="B22" s="3">
+        <v>1021</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="4">
-        <v>1021</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>32</v>
+      <c r="B23" s="1">
+        <v>1022</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="1">
-        <v>1022</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
+      <c r="B24" s="3">
+        <v>1023</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="4">
-        <v>1023</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>33</v>
+      <c r="B25" s="1">
+        <v>1024</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1151,22 +1144,22 @@
         <v>31</v>
       </c>
       <c r="B26" s="1">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -1175,34 +1168,34 @@
         <v>34</v>
       </c>
       <c r="B28" s="1">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="1">
-        <v>1027</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>6</v>
+      <c r="B29" s="3">
+        <v>1028</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="4">
-        <v>1028</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>35</v>
+      <c r="B30" s="1">
+        <v>1029</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D30" s="1"/>
     </row>
@@ -1211,7 +1204,7 @@
         <v>34</v>
       </c>
       <c r="B31" s="1">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
@@ -1223,10 +1216,10 @@
         <v>34</v>
       </c>
       <c r="B32" s="1">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D32" s="1"/>
     </row>
@@ -1235,7 +1228,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="1">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>8</v>
@@ -1243,38 +1236,38 @@
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="3">
-        <v>1032</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B34" s="1">
+        <v>1034</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B35" s="1">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D36" s="1"/>
     </row>
@@ -1283,10 +1276,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D37" s="1"/>
     </row>
@@ -1295,10 +1288,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="1">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D38" s="1"/>
     </row>
@@ -1307,7 +1300,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="1">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>6</v>
@@ -1319,22 +1312,22 @@
         <v>36</v>
       </c>
       <c r="B40" s="1">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="1">
-        <v>1039</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>6</v>
+      <c r="B41" s="3">
+        <v>1041</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="D41" s="1"/>
     </row>
@@ -1343,46 +1336,46 @@
         <v>36</v>
       </c>
       <c r="B42" s="1">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="4">
-        <v>1041</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>37</v>
+      <c r="B43" s="1">
+        <v>1043</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B44" s="1">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B45" s="1">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D45" s="1"/>
     </row>
@@ -1391,10 +1384,10 @@
         <v>38</v>
       </c>
       <c r="B46" s="1">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D46" s="1"/>
     </row>
@@ -1403,7 +1396,7 @@
         <v>38</v>
       </c>
       <c r="B47" s="1">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>6</v>
@@ -1415,22 +1408,22 @@
         <v>38</v>
       </c>
       <c r="B48" s="1">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D48" s="1"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B49" s="1">
-        <v>1047</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>6</v>
+      <c r="B49" s="3">
+        <v>1049</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="D49" s="1"/>
     </row>
@@ -1439,22 +1432,22 @@
         <v>38</v>
       </c>
       <c r="B50" s="1">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B51" s="4">
-        <v>1049</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>39</v>
+      <c r="B51" s="1">
+        <v>1051</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D51" s="1"/>
     </row>
@@ -1463,19 +1456,19 @@
         <v>38</v>
       </c>
       <c r="B52" s="1">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B53" s="1">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>6</v>
@@ -1484,10 +1477,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B54" s="1">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>6</v>
@@ -1499,22 +1492,22 @@
         <v>40</v>
       </c>
       <c r="B55" s="1">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B56" s="1">
-        <v>1054</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>6</v>
+      <c r="B56" s="3">
+        <v>1056</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D56" s="1"/>
     </row>
@@ -1523,22 +1516,22 @@
         <v>40</v>
       </c>
       <c r="B57" s="1">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B58" s="1">
+        <v>1058</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D57" s="1"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B58" s="4">
-        <v>1056</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="D58" s="1"/>
     </row>
@@ -1547,10 +1540,10 @@
         <v>40</v>
       </c>
       <c r="B59" s="1">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D59" s="1"/>
     </row>
@@ -1559,10 +1552,10 @@
         <v>40</v>
       </c>
       <c r="B60" s="1">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D60" s="1"/>
     </row>
@@ -1571,19 +1564,19 @@
         <v>40</v>
       </c>
       <c r="B61" s="1">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B62" s="1">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>6</v>
@@ -1591,14 +1584,14 @@
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B63" s="1">
-        <v>1061</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>6</v>
+      <c r="A63" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" s="3">
+        <v>1063</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="D63" s="1"/>
     </row>
@@ -1607,22 +1600,22 @@
         <v>42</v>
       </c>
       <c r="B64" s="1">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D64" s="1"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B65" s="4">
-        <v>1063</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>43</v>
+      <c r="B65" s="1">
+        <v>1065</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D65" s="1"/>
     </row>
@@ -1631,7 +1624,7 @@
         <v>42</v>
       </c>
       <c r="B66" s="1">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>8</v>
@@ -1643,7 +1636,7 @@
         <v>42</v>
       </c>
       <c r="B67" s="1">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>6</v>
@@ -1655,7 +1648,7 @@
         <v>42</v>
       </c>
       <c r="B68" s="1">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>8</v>
@@ -1667,7 +1660,7 @@
         <v>42</v>
       </c>
       <c r="B69" s="1">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>6</v>
@@ -1676,25 +1669,25 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B70" s="1">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B71" s="1">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D71" s="1"/>
     </row>
@@ -1703,7 +1696,7 @@
         <v>44</v>
       </c>
       <c r="B72" s="1">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>6</v>
@@ -1715,7 +1708,7 @@
         <v>44</v>
       </c>
       <c r="B73" s="1">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>8</v>
@@ -1727,7 +1720,7 @@
         <v>44</v>
       </c>
       <c r="B74" s="1">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>6</v>
@@ -1739,10 +1732,10 @@
         <v>44</v>
       </c>
       <c r="B75" s="1">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D75" s="1"/>
     </row>
@@ -1751,10 +1744,10 @@
         <v>44</v>
       </c>
       <c r="B76" s="1">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D76" s="1"/>
     </row>
@@ -1763,10 +1756,10 @@
         <v>44</v>
       </c>
       <c r="B77" s="1">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D77" s="1"/>
     </row>
@@ -1775,34 +1768,34 @@
         <v>44</v>
       </c>
       <c r="B78" s="1">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B79" s="1">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D79" s="1"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B80" s="1">
-        <v>1078</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>6</v>
+      <c r="A80" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B80" s="3">
+        <v>1080</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="D80" s="1"/>
     </row>
@@ -1811,70 +1804,70 @@
         <v>45</v>
       </c>
       <c r="B81" s="1">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D81" s="1"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="4" t="s">
+      <c r="A82" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B82" s="4">
-        <v>1080</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>46</v>
+      <c r="B82" s="1">
+        <v>1082</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D82" s="1"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B83" s="1">
-        <v>1081</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>6</v>
+      <c r="B83" s="3">
+        <v>1083</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="D83" s="1"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B84" s="1">
-        <v>1082</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>23</v>
+      <c r="B84" s="3">
+        <v>1084</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="D84" s="1"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B85" s="4">
-        <v>1083</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>47</v>
+      <c r="B85" s="1">
+        <v>1085</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D85" s="1"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="4" t="s">
+      <c r="A86" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B86" s="4">
-        <v>1084</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>48</v>
+      <c r="B86" s="1">
+        <v>1086</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D86" s="1"/>
     </row>
@@ -1883,7 +1876,7 @@
         <v>45</v>
       </c>
       <c r="B87" s="1">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>6</v>
@@ -1892,10 +1885,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B88" s="1">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>6</v>
@@ -1904,10 +1897,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B89" s="1">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>6</v>
@@ -1919,10 +1912,10 @@
         <v>49</v>
       </c>
       <c r="B90" s="1">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D90" s="1"/>
     </row>
@@ -1931,7 +1924,7 @@
         <v>49</v>
       </c>
       <c r="B91" s="1">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>6</v>
@@ -1943,10 +1936,10 @@
         <v>49</v>
       </c>
       <c r="B92" s="1">
-        <v>1090</v>
+        <v>1092</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D92" s="1"/>
     </row>
@@ -1955,7 +1948,7 @@
         <v>49</v>
       </c>
       <c r="B93" s="1">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>6</v>
@@ -1967,7 +1960,7 @@
         <v>49</v>
       </c>
       <c r="B94" s="1">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>6</v>
@@ -1979,7 +1972,7 @@
         <v>49</v>
       </c>
       <c r="B95" s="1">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>6</v>
@@ -1987,38 +1980,38 @@
       <c r="D95" s="1"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+      <c r="A96" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B96" s="1">
-        <v>1094</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>6</v>
+      <c r="B96" s="3">
+        <v>1096</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D96" s="1"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B97" s="1">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D97" s="1"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B98" s="4">
-        <v>1096</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>50</v>
+      <c r="A98" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B98" s="1">
+        <v>1098</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D98" s="1"/>
     </row>
@@ -2027,22 +2020,22 @@
         <v>51</v>
       </c>
       <c r="B99" s="1">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D99" s="1"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
+      <c r="A100" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B100" s="1">
-        <v>1098</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>6</v>
+      <c r="B100" s="3">
+        <v>1100</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="D100" s="1"/>
     </row>
@@ -2051,7 +2044,7 @@
         <v>51</v>
       </c>
       <c r="B101" s="1">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>6</v>
@@ -2059,26 +2052,26 @@
       <c r="D101" s="1"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="4" t="s">
+      <c r="A102" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B102" s="4">
-        <v>1100</v>
-      </c>
-      <c r="C102" s="4" t="s">
-        <v>52</v>
+      <c r="B102" s="1">
+        <v>1102</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D102" s="1"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
+      <c r="A103" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B103" s="1">
-        <v>1101</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>6</v>
+      <c r="B103" s="3">
+        <v>1103</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="D103" s="1"/>
     </row>
@@ -2087,106 +2080,106 @@
         <v>51</v>
       </c>
       <c r="B104" s="1">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D104" s="1"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B105" s="4">
-        <v>1103</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>53</v>
+      <c r="B105" s="1">
+        <v>1105</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D105" s="1"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B106" s="1">
-        <v>1104</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>6</v>
+      <c r="A106" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B106" s="3">
+        <v>1106</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="D106" s="1"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B107" s="1">
-        <v>1105</v>
+        <v>1107</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D107" s="1"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B108" s="4">
-        <v>1106</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>55</v>
+      <c r="A108" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B108" s="1">
+        <v>1108</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
+      <c r="A109" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B109" s="1">
-        <v>1107</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>8</v>
+      <c r="B109" s="3">
+        <v>1109</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
+      <c r="A110" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B110" s="1">
-        <v>1108</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>6</v>
+      <c r="B110" s="3">
+        <v>1110</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="D110" s="1"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="4" t="s">
+      <c r="A111" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B111" s="4">
-        <v>1109</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>47</v>
+      <c r="B111" s="1">
+        <v>1111</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D111" s="1"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="4" t="s">
+      <c r="A112" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B112" s="4">
-        <v>1110</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>57</v>
+      <c r="B112" s="1">
+        <v>1112</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D112" s="1"/>
     </row>
@@ -2195,10 +2188,10 @@
         <v>56</v>
       </c>
       <c r="B113" s="1">
-        <v>1111</v>
+        <v>1113</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D113" s="1"/>
     </row>
@@ -2207,7 +2200,7 @@
         <v>56</v>
       </c>
       <c r="B114" s="1">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>6</v>
@@ -2216,22 +2209,22 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B115" s="1">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D115" s="1"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B116" s="1">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>6</v>
@@ -2243,10 +2236,10 @@
         <v>58</v>
       </c>
       <c r="B117" s="1">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D117" s="1"/>
     </row>
@@ -2255,7 +2248,7 @@
         <v>58</v>
       </c>
       <c r="B118" s="1">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>6</v>
@@ -2267,10 +2260,10 @@
         <v>58</v>
       </c>
       <c r="B119" s="1">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D119" s="1"/>
     </row>
@@ -2279,7 +2272,7 @@
         <v>58</v>
       </c>
       <c r="B120" s="1">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>6</v>
@@ -2291,10 +2284,10 @@
         <v>58</v>
       </c>
       <c r="B121" s="1">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D121" s="1"/>
     </row>
@@ -2303,7 +2296,7 @@
         <v>58</v>
       </c>
       <c r="B122" s="1">
-        <v>1120</v>
+        <v>1122</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>6</v>
@@ -2315,34 +2308,34 @@
         <v>58</v>
       </c>
       <c r="B123" s="1">
-        <v>1121</v>
+        <v>1123</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D123" s="1"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B124" s="1">
-        <v>1122</v>
+        <v>1124</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D124" s="1"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B125" s="1">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D125" s="1"/>
     </row>
@@ -2351,22 +2344,22 @@
         <v>59</v>
       </c>
       <c r="B126" s="1">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D126" s="1"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
+      <c r="A127" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B127" s="1">
-        <v>1125</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>6</v>
+      <c r="B127" s="3">
+        <v>1127</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="D127" s="1"/>
     </row>
@@ -2375,22 +2368,22 @@
         <v>59</v>
       </c>
       <c r="B128" s="1">
-        <v>1126</v>
+        <v>1128</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D128" s="1"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" s="4" t="s">
+      <c r="A129" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B129" s="4">
-        <v>1127</v>
-      </c>
-      <c r="C129" s="4" t="s">
-        <v>47</v>
+      <c r="B129" s="3">
+        <v>1129</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="D129" s="1"/>
     </row>
@@ -2399,22 +2392,22 @@
         <v>59</v>
       </c>
       <c r="B130" s="1">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c r="C130" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D130" s="1"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B131" s="1">
+        <v>1131</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D130" s="1"/>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B131" s="4">
-        <v>1129</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="D131" s="1"/>
     </row>
@@ -2423,34 +2416,34 @@
         <v>59</v>
       </c>
       <c r="B132" s="1">
-        <v>1130</v>
+        <v>1132</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D132" s="1"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B133" s="1">
-        <v>1131</v>
+        <v>1133</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D133" s="1"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B134" s="1">
-        <v>1132</v>
+        <v>1134</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D134" s="1"/>
     </row>
@@ -2459,10 +2452,10 @@
         <v>61</v>
       </c>
       <c r="B135" s="1">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D135" s="1"/>
     </row>
@@ -2471,7 +2464,7 @@
         <v>61</v>
       </c>
       <c r="B136" s="1">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>6</v>
@@ -2483,10 +2476,10 @@
         <v>61</v>
       </c>
       <c r="B137" s="1">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D137" s="1"/>
     </row>
@@ -2495,10 +2488,10 @@
         <v>61</v>
       </c>
       <c r="B138" s="1">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D138" s="1"/>
     </row>
@@ -2507,7 +2500,7 @@
         <v>61</v>
       </c>
       <c r="B139" s="1">
-        <v>1137</v>
+        <v>1139</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>6</v>
@@ -2519,10 +2512,10 @@
         <v>61</v>
       </c>
       <c r="B140" s="1">
-        <v>1138</v>
+        <v>1140</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D140" s="1"/>
     </row>
@@ -2531,34 +2524,34 @@
         <v>61</v>
       </c>
       <c r="B141" s="1">
-        <v>1139</v>
+        <v>1141</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D141" s="1"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B142" s="1">
-        <v>1140</v>
+        <v>1142</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D142" s="1"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B143" s="1">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D143" s="1"/>
     </row>
@@ -2567,10 +2560,10 @@
         <v>62</v>
       </c>
       <c r="B144" s="1">
-        <v>1142</v>
+        <v>1144</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D144" s="1"/>
     </row>
@@ -2579,10 +2572,10 @@
         <v>62</v>
       </c>
       <c r="B145" s="1">
-        <v>1143</v>
+        <v>1145</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D145" s="1"/>
     </row>
@@ -2591,10 +2584,10 @@
         <v>62</v>
       </c>
       <c r="B146" s="1">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D146" s="1"/>
     </row>
@@ -2603,7 +2596,7 @@
         <v>62</v>
       </c>
       <c r="B147" s="1">
-        <v>1145</v>
+        <v>1147</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>10</v>
@@ -2612,25 +2605,25 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B148" s="1">
-        <v>1146</v>
+        <v>1148</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D148" s="1"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B149" s="1">
-        <v>1147</v>
+        <v>1149</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D149" s="1"/>
     </row>
@@ -2639,10 +2632,10 @@
         <v>63</v>
       </c>
       <c r="B150" s="1">
-        <v>1148</v>
+        <v>1150</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D150" s="1"/>
     </row>
@@ -2651,7 +2644,7 @@
         <v>63</v>
       </c>
       <c r="B151" s="1">
-        <v>1149</v>
+        <v>1151</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>6</v>
@@ -2663,22 +2656,22 @@
         <v>63</v>
       </c>
       <c r="B152" s="1">
-        <v>1150</v>
+        <v>1152</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D152" s="1"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A153" s="1" t="s">
+      <c r="A153" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B153" s="1">
-        <v>1151</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>6</v>
+      <c r="B153" s="3">
+        <v>1153</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="D153" s="1"/>
     </row>
@@ -2687,22 +2680,22 @@
         <v>63</v>
       </c>
       <c r="B154" s="1">
-        <v>1152</v>
+        <v>1154</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D154" s="1"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A155" s="4" t="s">
+      <c r="A155" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B155" s="4">
-        <v>1153</v>
-      </c>
-      <c r="C155" s="4" t="s">
-        <v>64</v>
+      <c r="B155" s="1">
+        <v>1155</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D155" s="1"/>
     </row>
@@ -2711,31 +2704,31 @@
         <v>63</v>
       </c>
       <c r="B156" s="1">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D156" s="1"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B157" s="1">
-        <v>1155</v>
+        <v>1157</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D157" s="1"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B158" s="1">
-        <v>1156</v>
+        <v>1158</v>
       </c>
       <c r="C158" s="1" t="s">
         <v>6</v>
@@ -2747,10 +2740,10 @@
         <v>65</v>
       </c>
       <c r="B159" s="1">
-        <v>1157</v>
+        <v>1159</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D159" s="1"/>
     </row>
@@ -2759,7 +2752,7 @@
         <v>65</v>
       </c>
       <c r="B160" s="1">
-        <v>1158</v>
+        <v>1160</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>6</v>
@@ -2771,10 +2764,10 @@
         <v>65</v>
       </c>
       <c r="B161" s="1">
-        <v>1159</v>
+        <v>1161</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D161" s="1"/>
     </row>
@@ -2783,7 +2776,7 @@
         <v>65</v>
       </c>
       <c r="B162" s="1">
-        <v>1160</v>
+        <v>1162</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>6</v>
@@ -2795,10 +2788,10 @@
         <v>65</v>
       </c>
       <c r="B163" s="1">
-        <v>1161</v>
+        <v>1163</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D163" s="1"/>
     </row>
@@ -2807,7 +2800,7 @@
         <v>65</v>
       </c>
       <c r="B164" s="1">
-        <v>1162</v>
+        <v>1164</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>6</v>
@@ -2819,7 +2812,7 @@
         <v>65</v>
       </c>
       <c r="B165" s="1">
-        <v>1163</v>
+        <v>1165</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>6</v>
@@ -2828,10 +2821,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B166" s="1">
-        <v>1164</v>
+        <v>1166</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>6</v>
@@ -2840,13 +2833,13 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B167" s="1">
-        <v>1165</v>
+        <v>1167</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D167" s="1"/>
     </row>
@@ -2855,7 +2848,7 @@
         <v>66</v>
       </c>
       <c r="B168" s="1">
-        <v>1166</v>
+        <v>1168</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>6</v>
@@ -2867,10 +2860,10 @@
         <v>66</v>
       </c>
       <c r="B169" s="1">
-        <v>1167</v>
+        <v>1169</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D169" s="1"/>
     </row>
@@ -2879,7 +2872,7 @@
         <v>66</v>
       </c>
       <c r="B170" s="1">
-        <v>1168</v>
+        <v>1170</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>6</v>
@@ -2891,7 +2884,7 @@
         <v>66</v>
       </c>
       <c r="B171" s="1">
-        <v>1169</v>
+        <v>1171</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>6</v>
@@ -2903,7 +2896,7 @@
         <v>66</v>
       </c>
       <c r="B172" s="1">
-        <v>1170</v>
+        <v>1172</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>6</v>
@@ -2915,10 +2908,10 @@
         <v>66</v>
       </c>
       <c r="B173" s="1">
-        <v>1171</v>
+        <v>1173</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D173" s="1"/>
     </row>
@@ -2927,7 +2920,7 @@
         <v>66</v>
       </c>
       <c r="B174" s="1">
-        <v>1172</v>
+        <v>1174</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>6</v>
@@ -2936,22 +2929,22 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B175" s="1">
-        <v>1173</v>
+        <v>1175</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D175" s="1"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B176" s="1">
-        <v>1174</v>
+        <v>1176</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>6</v>
@@ -2963,7 +2956,7 @@
         <v>67</v>
       </c>
       <c r="B177" s="1">
-        <v>1175</v>
+        <v>1177</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>8</v>
@@ -2975,7 +2968,7 @@
         <v>67</v>
       </c>
       <c r="B178" s="1">
-        <v>1176</v>
+        <v>1178</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>6</v>
@@ -2987,10 +2980,10 @@
         <v>67</v>
       </c>
       <c r="B179" s="1">
-        <v>1177</v>
+        <v>1179</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D179" s="1"/>
     </row>
@@ -2999,7 +2992,7 @@
         <v>67</v>
       </c>
       <c r="B180" s="1">
-        <v>1178</v>
+        <v>1180</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>6</v>
@@ -3011,10 +3004,10 @@
         <v>67</v>
       </c>
       <c r="B181" s="1">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D181" s="1"/>
     </row>
@@ -3023,19 +3016,19 @@
         <v>67</v>
       </c>
       <c r="B182" s="1">
-        <v>1180</v>
+        <v>1182</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D182" s="1"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B183" s="1">
-        <v>1181</v>
+        <v>1183</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>6</v>
@@ -3044,13 +3037,13 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B184" s="1">
-        <v>1182</v>
+        <v>1184</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D184" s="1"/>
     </row>
@@ -3059,10 +3052,10 @@
         <v>68</v>
       </c>
       <c r="B185" s="1">
-        <v>1183</v>
+        <v>1185</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D185" s="1"/>
     </row>
@@ -3071,10 +3064,10 @@
         <v>68</v>
       </c>
       <c r="B186" s="1">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D186" s="1"/>
     </row>
@@ -3083,10 +3076,10 @@
         <v>68</v>
       </c>
       <c r="B187" s="1">
-        <v>1185</v>
+        <v>1187</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D187" s="1"/>
     </row>
@@ -3095,10 +3088,10 @@
         <v>68</v>
       </c>
       <c r="B188" s="1">
-        <v>1186</v>
+        <v>1188</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D188" s="1"/>
     </row>
@@ -3107,55 +3100,31 @@
         <v>68</v>
       </c>
       <c r="B189" s="1">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D189" s="1"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B190" s="1">
-        <v>1188</v>
+        <v>1190</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D190" s="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B191" s="1">
-        <v>1189</v>
+        <v>1191</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A192" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B192" s="1">
-        <v>1190</v>
-      </c>
-      <c r="C192" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A193" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B193" s="1">
-        <v>1191</v>
-      </c>
-      <c r="C193" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3165,6 +3134,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD172B1A8CFBF549BD23145C0D4C69AA" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60d392b449e0a1bb062ed007359ef7f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="98201be9-bed6-4c9e-8a9b-8dbdcb59b52e" xmlns:ns4="eb7b1eea-95e0-4f99-a517-75d51ebb206f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f35683e864675bf732228debc427d31" ns3:_="" ns4:_="">
     <xsd:import namespace="98201be9-bed6-4c9e-8a9b-8dbdcb59b52e"/>
@@ -3393,15 +3371,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3411,6 +3380,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DC39010-99A4-420F-8930-47F0BD8B70E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA519E84-2031-44C1-A446-0F69C93EE441}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3425,14 +3402,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DC39010-99A4-420F-8930-47F0BD8B70E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>